<commit_message>
updated version of data dictionary
</commit_message>
<xml_diff>
--- a/emit_nat_2012_2013_df_dict.xlsx
+++ b/emit_nat_2012_2013_df_dict.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobbuenodemesquita/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobbuenodemesquita/Desktop/git_repos/emit_umd_natural_infection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E37D34-0FCA-2D41-BBFE-18D8BBA6A43D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B30944-5646-1D42-9BE6-0F55DD1B3DD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38380" yWindow="460" windowWidth="38380" windowHeight="21140" xr2:uid="{C8699F27-9584-2943-BFF6-70E2238E4631}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>variable</t>
   </si>
@@ -331,6 +331,24 @@
   </si>
   <si>
     <t>G2 elbow temperature in degrees F</t>
+  </si>
+  <si>
+    <t>upper_sx</t>
+  </si>
+  <si>
+    <t>lower_sx</t>
+  </si>
+  <si>
+    <t>systemic_sx</t>
+  </si>
+  <si>
+    <t>nose_run + nose_stuf + sneeze + throat_sr + earache (as implemented in Yan et al., 2018 PNAS https://www.pnas.org/content/115/5/1081)</t>
+  </si>
+  <si>
+    <t>chest_tight + sob + cough (as implemented in Yan et al., 2018 PNAS https://www.pnas.org/content/115/5/1081)</t>
+  </si>
+  <si>
+    <t>malaise + headache + mj_ache + lymph_node + sw_fever_chill (as implemented in Yan et al., 2018 PNAS https://www.pnas.org/content/115/5/1081)</t>
   </si>
 </sst>
 </file>
@@ -691,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA514D55-2733-0F48-B8EE-9AF6C5C913E4}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1111,6 +1129,30 @@
         <v>75</v>
       </c>
     </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>